<commit_message>
update main table 2 (comp. effect direction, round numbers)
</commit_message>
<xml_diff>
--- a/tables/MainTable2.xlsx
+++ b/tables/MainTable2.xlsx
@@ -11,15 +11,15 @@
     <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Description!$A$1:$B$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table2!$A$1:$I$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Description!$A$1:$B$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table2!$A$1:$J$9</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>regions</t>
   </si>
@@ -36,6 +36,9 @@
     <t>bestSettings</t>
   </si>
   <si>
+    <t>discordantEffect</t>
+  </si>
+  <si>
     <t>LD_r2</t>
   </si>
   <si>
@@ -63,6 +66,9 @@
     <t>MALE, ALL</t>
   </si>
   <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
@@ -121,6 +127,9 @@
   </si>
   <si>
     <t>rs112708523</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
   <si>
     <t>14, 21</t>
@@ -518,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -527,7 +536,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,248 +564,275 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>0.902592</v>
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
       </c>
       <c r="G2">
-        <v>0.725061250565889</v>
+        <v>0.9</v>
       </c>
       <c r="H2">
-        <v>0.274550778799065</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0.73</v>
+      </c>
+      <c r="I2">
+        <v>0.27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.75</v>
+      </c>
+      <c r="I3">
+        <v>0.25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>0.02</v>
+      </c>
+      <c r="H4">
+        <v>0.99</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>0.96</v>
+      </c>
+      <c r="H5">
+        <v>0.07</v>
+      </c>
+      <c r="I5">
+        <v>0.93</v>
+      </c>
+      <c r="J5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3">
-        <v>0.000814754</v>
-      </c>
-      <c r="G3">
-        <v>0.750809203825439</v>
-      </c>
-      <c r="H3">
-        <v>0.249188184373361</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>0.28</v>
+      </c>
+      <c r="H6">
+        <v>0.45</v>
+      </c>
+      <c r="I6">
+        <v>0.54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7">
+        <v>0.98</v>
+      </c>
+      <c r="H7">
+        <v>0.47</v>
+      </c>
+      <c r="I7">
+        <v>0.53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>0.99</v>
+      </c>
+      <c r="H8">
+        <v>0.48</v>
+      </c>
+      <c r="I8">
+        <v>0.52</v>
+      </c>
+      <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <v>0.0162103</v>
-      </c>
-      <c r="G4">
-        <v>0.99342668756948</v>
-      </c>
-      <c r="H4">
-        <v>0.0032732707544401</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5">
-        <v>0.960124</v>
-      </c>
-      <c r="G5">
-        <v>0.067762569387176</v>
-      </c>
-      <c r="H5">
-        <v>0.932227681333968</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6">
-        <v>0.278674</v>
-      </c>
-      <c r="G6">
-        <v>0.452639692291773</v>
-      </c>
-      <c r="H6">
-        <v>0.535680058893856</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>0.978384</v>
-      </c>
-      <c r="G7">
-        <v>0.469578982059398</v>
-      </c>
-      <c r="H7">
-        <v>0.530420963356273</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8">
-        <v>0.985336</v>
-      </c>
-      <c r="G8">
-        <v>0.479309795438985</v>
-      </c>
-      <c r="H8">
-        <v>0.518136381133117</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>1.00024</v>
-      </c>
-      <c r="G9">
-        <v>0.0011257034394452</v>
-      </c>
-      <c r="H9">
-        <v>0.998874296560553</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I9"/>
+  <autoFilter ref="A1:J9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -807,10 +843,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -818,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -826,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -834,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -842,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -850,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -858,7 +894,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -866,7 +902,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -874,7 +910,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -882,11 +918,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10"/>
+  <autoFilter ref="A1:B11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>